<commit_message>
Added level 8 to the game
</commit_message>
<xml_diff>
--- a/Base/TileMap/Level8.xlsx
+++ b/Base/TileMap/Level8.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xecli\Documents\Git\Base\TileMap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xecli\Documents\Git\-SP3-Lone-Spectre.git\Base\TileMap\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -555,7 +555,591 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="74">
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -664,33 +1248,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -972,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BE17" sqref="BE17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,7 +2069,7 @@
         <v>0</v>
       </c>
       <c r="AV3" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AW3" s="1">
         <v>1</v>
@@ -2679,16 +3236,16 @@
         <v>0</v>
       </c>
       <c r="AW9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA9" s="1">
         <v>1</v>
@@ -2873,19 +3430,19 @@
         <v>0</v>
       </c>
       <c r="AW10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB10" s="1">
         <v>1</v>
@@ -3058,31 +3615,31 @@
         <v>1</v>
       </c>
       <c r="AT11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV11" s="1">
         <v>17</v>
       </c>
-      <c r="AU11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV11" s="1">
-        <v>0</v>
-      </c>
       <c r="AW11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC11" s="1">
         <v>1</v>
@@ -3255,10 +3812,10 @@
         <v>1</v>
       </c>
       <c r="AU12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW12" s="1">
         <v>1</v>
@@ -3273,10 +3830,10 @@
         <v>1</v>
       </c>
       <c r="BA12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC12" s="1">
         <v>1</v>
@@ -3449,10 +4006,10 @@
         <v>1</v>
       </c>
       <c r="AU13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW13" s="1">
         <v>1</v>
@@ -3467,10 +4024,10 @@
         <v>1</v>
       </c>
       <c r="BA13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC13" s="1">
         <v>1</v>
@@ -3640,31 +4197,31 @@
         <v>1</v>
       </c>
       <c r="AT14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU14" s="1">
         <v>22</v>
       </c>
-      <c r="AU14" s="1">
-        <v>0</v>
-      </c>
       <c r="AV14" s="1">
         <v>0</v>
       </c>
       <c r="AW14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC14" s="1">
         <v>1</v>
@@ -3837,28 +4394,28 @@
         <v>1</v>
       </c>
       <c r="AU15" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AV15" s="1">
         <v>0</v>
       </c>
       <c r="AW15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC15" s="1">
         <v>1</v>
@@ -4037,16 +4594,16 @@
         <v>0</v>
       </c>
       <c r="AW16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA16" s="1">
         <v>1</v>
@@ -4425,7 +4982,7 @@
         <v>0</v>
       </c>
       <c r="AW18" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="AX18" s="1">
         <v>1</v>
@@ -4813,7 +5370,7 @@
         <v>0</v>
       </c>
       <c r="AW20" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AX20" s="1">
         <v>1</v>
@@ -5007,7 +5564,7 @@
         <v>0</v>
       </c>
       <c r="AW21" s="1">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="AX21" s="1">
         <v>1</v>
@@ -5329,10 +5886,10 @@
         <v>1</v>
       </c>
       <c r="AA23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC23" s="1">
         <v>1</v>
@@ -5389,10 +5946,10 @@
         <v>1</v>
       </c>
       <c r="AU23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW23" s="1">
         <v>1</v>
@@ -5523,10 +6080,10 @@
         <v>1</v>
       </c>
       <c r="AA24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC24" s="1">
         <v>1</v>
@@ -5583,10 +6140,10 @@
         <v>1</v>
       </c>
       <c r="AU24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW24" s="1">
         <v>1</v>
@@ -5717,10 +6274,10 @@
         <v>1</v>
       </c>
       <c r="AA25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC25" s="1">
         <v>1</v>
@@ -5777,10 +6334,10 @@
         <v>1</v>
       </c>
       <c r="AU25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW25" s="1">
         <v>1</v>
@@ -5890,25 +6447,25 @@
         <v>1</v>
       </c>
       <c r="T26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA26" s="1">
         <v>0</v>
@@ -5917,64 +6474,64 @@
         <v>0</v>
       </c>
       <c r="AC26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH26" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="AI26" s="1">
         <v>1</v>
       </c>
       <c r="AJ26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW26" s="1">
         <v>1</v>
@@ -6084,25 +6641,25 @@
         <v>1</v>
       </c>
       <c r="T27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA27" s="1">
         <v>0</v>
@@ -6111,64 +6668,64 @@
         <v>0</v>
       </c>
       <c r="AC27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW27" s="1">
         <v>1</v>
@@ -6278,91 +6835,91 @@
         <v>1</v>
       </c>
       <c r="T28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW28" s="1">
         <v>1</v>
@@ -6487,10 +7044,10 @@
         <v>1</v>
       </c>
       <c r="Y29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA29" s="1">
         <v>1</v>
@@ -6511,13 +7068,13 @@
         <v>1</v>
       </c>
       <c r="AG29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH29" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AI29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ29" s="1">
         <v>1</v>
@@ -6538,10 +7095,10 @@
         <v>1</v>
       </c>
       <c r="AP29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR29" s="1">
         <v>1</v>
@@ -6681,10 +7238,10 @@
         <v>1</v>
       </c>
       <c r="Y30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA30" s="1">
         <v>1</v>
@@ -6705,13 +7262,13 @@
         <v>1</v>
       </c>
       <c r="AG30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ30" s="1">
         <v>1</v>
@@ -6732,10 +7289,10 @@
         <v>1</v>
       </c>
       <c r="AP30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR30" s="1">
         <v>1</v>
@@ -6869,22 +7426,22 @@
         <v>1</v>
       </c>
       <c r="W31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC31" s="1">
         <v>1</v>
@@ -6899,13 +7456,13 @@
         <v>1</v>
       </c>
       <c r="AG31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ31" s="1">
         <v>1</v>
@@ -6920,22 +7477,22 @@
         <v>1</v>
       </c>
       <c r="AN31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT31" s="1">
         <v>1</v>
@@ -7063,22 +7620,22 @@
         <v>1</v>
       </c>
       <c r="W32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC32" s="1">
         <v>1</v>
@@ -7093,13 +7650,13 @@
         <v>1</v>
       </c>
       <c r="AG32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ32" s="1">
         <v>1</v>
@@ -7114,22 +7671,22 @@
         <v>1</v>
       </c>
       <c r="AN32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT32" s="1">
         <v>1</v>
@@ -7200,46 +7757,46 @@
         <v>1</v>
       </c>
       <c r="D33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R33" s="1">
         <v>1</v>
@@ -7257,22 +7814,22 @@
         <v>1</v>
       </c>
       <c r="W33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC33" s="1">
         <v>1</v>
@@ -7287,13 +7844,13 @@
         <v>1</v>
       </c>
       <c r="AG33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ33" s="1">
         <v>1</v>
@@ -7308,22 +7865,22 @@
         <v>1</v>
       </c>
       <c r="AN33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT33" s="1">
         <v>1</v>
@@ -7391,52 +7948,52 @@
         <v>1</v>
       </c>
       <c r="C34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S34" s="1">
         <v>1</v>
@@ -7451,22 +8008,22 @@
         <v>1</v>
       </c>
       <c r="W34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC34" s="1">
         <v>1</v>
@@ -7481,13 +8038,13 @@
         <v>1</v>
       </c>
       <c r="AG34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ34" s="1">
         <v>1</v>
@@ -7502,22 +8059,22 @@
         <v>1</v>
       </c>
       <c r="AN34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT34" s="1">
         <v>1</v>
@@ -7585,52 +8142,52 @@
         <v>1</v>
       </c>
       <c r="C35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S35" s="1">
         <v>1</v>
@@ -7645,22 +8202,22 @@
         <v>1</v>
       </c>
       <c r="W35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC35" s="1">
         <v>1</v>
@@ -7675,13 +8232,13 @@
         <v>1</v>
       </c>
       <c r="AG35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ35" s="1">
         <v>1</v>
@@ -7696,22 +8253,22 @@
         <v>1</v>
       </c>
       <c r="AN35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT35" s="1">
         <v>1</v>
@@ -7779,52 +8336,52 @@
         <v>1</v>
       </c>
       <c r="C36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S36" s="1">
         <v>1</v>
@@ -7839,22 +8396,22 @@
         <v>1</v>
       </c>
       <c r="W36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC36" s="1">
         <v>1</v>
@@ -7869,13 +8426,13 @@
         <v>1</v>
       </c>
       <c r="AG36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ36" s="1">
         <v>1</v>
@@ -7890,22 +8447,22 @@
         <v>1</v>
       </c>
       <c r="AN36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT36" s="1">
         <v>1</v>
@@ -7973,52 +8530,52 @@
         <v>1</v>
       </c>
       <c r="C37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S37" s="1">
         <v>1</v>
@@ -8063,13 +8620,13 @@
         <v>1</v>
       </c>
       <c r="AG37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ37" s="1">
         <v>1</v>
@@ -8167,52 +8724,52 @@
         <v>1</v>
       </c>
       <c r="C38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S38" s="1">
         <v>1</v>
@@ -8245,37 +8802,37 @@
         <v>1</v>
       </c>
       <c r="AC38" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="AD38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM38" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="AN38" s="1">
         <v>1</v>
@@ -8361,52 +8918,52 @@
         <v>1</v>
       </c>
       <c r="C39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S39" s="1">
         <v>1</v>
@@ -8439,37 +8996,37 @@
         <v>1</v>
       </c>
       <c r="AC39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN39" s="1">
         <v>1</v>
@@ -8555,52 +9112,52 @@
         <v>1</v>
       </c>
       <c r="C40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S40" s="1">
         <v>1</v>
@@ -8612,31 +9169,31 @@
         <v>1</v>
       </c>
       <c r="V40" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="W40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB40" s="1">
         <v>1</v>
       </c>
       <c r="AC40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE40" s="1">
         <v>1</v>
@@ -8660,43 +9217,43 @@
         <v>1</v>
       </c>
       <c r="AL40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN40" s="1">
         <v>1</v>
       </c>
       <c r="AO40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY40" s="1">
         <v>1</v>
@@ -8749,52 +9306,52 @@
         <v>1</v>
       </c>
       <c r="C41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S41" s="1">
         <v>1</v>
@@ -8806,31 +9363,31 @@
         <v>1</v>
       </c>
       <c r="V41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB41" s="1">
         <v>1</v>
       </c>
       <c r="AC41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE41" s="1">
         <v>1</v>
@@ -8854,34 +9411,34 @@
         <v>1</v>
       </c>
       <c r="AL41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN41" s="1">
         <v>1</v>
       </c>
       <c r="AO41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV41" s="1">
         <v>1</v>
@@ -8890,7 +9447,7 @@
         <v>1</v>
       </c>
       <c r="AX41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY41" s="1">
         <v>1</v>
@@ -8943,52 +9500,52 @@
         <v>1</v>
       </c>
       <c r="C42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S42" s="1">
         <v>1</v>
@@ -9000,67 +9557,67 @@
         <v>1</v>
       </c>
       <c r="V42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X42" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="Y42" s="1">
         <v>1</v>
       </c>
       <c r="Z42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ42" s="1">
         <v>1</v>
@@ -9075,16 +9632,16 @@
         <v>1</v>
       </c>
       <c r="AU42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY42" s="1">
         <v>1</v>
@@ -9137,52 +9694,52 @@
         <v>1</v>
       </c>
       <c r="C43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S43" s="1">
         <v>1</v>
@@ -9194,10 +9751,10 @@
         <v>1</v>
       </c>
       <c r="V43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X43" s="1">
         <v>1</v>
@@ -9269,16 +9826,16 @@
         <v>1</v>
       </c>
       <c r="AU43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY43" s="1">
         <v>1</v>
@@ -9331,52 +9888,52 @@
         <v>1</v>
       </c>
       <c r="C44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S44" s="1">
         <v>1</v>
@@ -9388,10 +9945,10 @@
         <v>1</v>
       </c>
       <c r="V44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X44" s="1">
         <v>1</v>
@@ -9406,43 +9963,43 @@
         <v>1</v>
       </c>
       <c r="AB44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO44" s="1">
         <v>1</v>
@@ -9463,16 +10020,16 @@
         <v>1</v>
       </c>
       <c r="AU44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY44" s="1">
         <v>1</v>
@@ -9525,52 +10082,52 @@
         <v>1</v>
       </c>
       <c r="C45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S45" s="1">
         <v>1</v>
@@ -9582,13 +10139,13 @@
         <v>1</v>
       </c>
       <c r="V45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X45" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="Y45" s="1">
         <v>1</v>
@@ -9603,10 +10160,10 @@
         <v>1</v>
       </c>
       <c r="AC45" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AD45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE45" s="1">
         <v>1</v>
@@ -9624,10 +10181,10 @@
         <v>1</v>
       </c>
       <c r="AJ45" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="AK45" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AL45" s="1">
         <v>1</v>
@@ -9636,7 +10193,7 @@
         <v>1</v>
       </c>
       <c r="AN45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO45" s="1">
         <v>1</v>
@@ -9657,16 +10214,16 @@
         <v>1</v>
       </c>
       <c r="AU45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV45" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AW45" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AX45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY45" s="1">
         <v>1</v>
@@ -9719,52 +10276,52 @@
         <v>1</v>
       </c>
       <c r="C46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S46" s="1">
         <v>1</v>
@@ -9776,10 +10333,10 @@
         <v>1</v>
       </c>
       <c r="V46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X46" s="1">
         <v>1</v>
@@ -9800,7 +10357,7 @@
         <v>1</v>
       </c>
       <c r="AD46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE46" s="1">
         <v>1</v>
@@ -9815,22 +10372,22 @@
         <v>1</v>
       </c>
       <c r="AI46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO46" s="1">
         <v>1</v>
@@ -9851,16 +10408,16 @@
         <v>1</v>
       </c>
       <c r="AU46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY46" s="1">
         <v>1</v>
@@ -9913,52 +10470,52 @@
         <v>1</v>
       </c>
       <c r="C47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S47" s="1">
         <v>1</v>
@@ -9970,10 +10527,10 @@
         <v>1</v>
       </c>
       <c r="V47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X47" s="1">
         <v>1</v>
@@ -9994,7 +10551,7 @@
         <v>1</v>
       </c>
       <c r="AD47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE47" s="1">
         <v>1</v>
@@ -10024,37 +10581,37 @@
         <v>1</v>
       </c>
       <c r="AN47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO47" s="1">
         <v>1</v>
       </c>
       <c r="AP47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY47" s="1">
         <v>1</v>
@@ -10107,52 +10664,52 @@
         <v>1</v>
       </c>
       <c r="C48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S48" s="1">
         <v>1</v>
@@ -10164,13 +10721,13 @@
         <v>1</v>
       </c>
       <c r="V48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X48" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="Y48" s="1">
         <v>1</v>
@@ -10185,10 +10742,10 @@
         <v>1</v>
       </c>
       <c r="AC48" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AD48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE48" s="1">
         <v>1</v>
@@ -10218,7 +10775,7 @@
         <v>1</v>
       </c>
       <c r="AN48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO48" s="1">
         <v>1</v>
@@ -10227,7 +10784,7 @@
         <v>1</v>
       </c>
       <c r="AQ48" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="AR48" s="1">
         <v>1</v>
@@ -10239,16 +10796,16 @@
         <v>1</v>
       </c>
       <c r="AU48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY48" s="1">
         <v>1</v>
@@ -10304,46 +10861,46 @@
         <v>1</v>
       </c>
       <c r="D49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R49" s="1">
         <v>1</v>
@@ -10355,34 +10912,34 @@
         <v>1</v>
       </c>
       <c r="U49" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="V49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE49" s="1">
         <v>1</v>
@@ -10406,34 +10963,34 @@
         <v>1</v>
       </c>
       <c r="AL49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV49" s="1">
         <v>1</v>
@@ -10442,7 +10999,7 @@
         <v>1</v>
       </c>
       <c r="AX49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY49" s="1">
         <v>1</v>
@@ -10615,7 +11172,7 @@
         <v>1</v>
       </c>
       <c r="AQ50" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AR50" s="1">
         <v>1</v>
@@ -10627,16 +11184,16 @@
         <v>1</v>
       </c>
       <c r="AU50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY50" s="1">
         <v>1</v>
@@ -10877,57 +11434,70 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="13" operator="between">
       <formula>15</formula>
       <formula>18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
       <formula>22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:BL51">
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
       <formula>-1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+      <formula>26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="between">
       <formula>15</formula>
       <formula>18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
       <formula>22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U17">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
-      <formula>15</formula>
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="between">
+      <formula>14</formula>
       <formula>18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U17">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="T49">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V49">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+      <formula>26</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>